<commit_message>
new splitsy by Knuth + PZ
</commit_message>
<xml_diff>
--- a/excel/parallel.xlsx
+++ b/excel/parallel.xlsx
@@ -30,8 +30,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="[h]:mm:ss;@"/>
-    <numFmt numFmtId="172" formatCode="mm:ss.000"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="165" formatCode="mm:ss.000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -65,12 +65,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -102,22 +102,31 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1'!$C$20:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1'!$A$8:$D$8</c:f>
+              <c:f>'1'!$C$8:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>mm:ss.000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.7777777777777781E-7</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.7199074074074075E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7500000000000006E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.7199074074074075E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>2.8718518518518519E-4</c:v>
                 </c:pt>
               </c:numCache>
@@ -138,22 +147,31 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1'!$C$20:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1'!$A$17:$D$17</c:f>
+              <c:f>'1'!$C$17:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>mm:ss.000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>6.1574074074074065E-7</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.8564814814814816E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2685185185185195E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.8564814814814816E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>2.7318981481481481E-4</c:v>
                 </c:pt>
               </c:numCache>
@@ -174,22 +192,31 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1'!$C$20:$D$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1'!$A$26:$D$26</c:f>
+              <c:f>'1'!$C$26:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>mm:ss.000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.6157407407407408E-7</c:v>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.953703703703704E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.4444444444444444E-7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.953703703703704E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>1.393240740740741E-4</c:v>
                 </c:pt>
               </c:numCache>
@@ -197,24 +224,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96484736"/>
-        <c:axId val="55661696"/>
+        <c:axId val="123320192"/>
+        <c:axId val="123321728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96484736"/>
+        <c:axId val="123320192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55661696"/>
+        <c:crossAx val="123321728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55661696"/>
+        <c:axId val="123321728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -222,7 +250,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="mm:ss.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96484736"/>
+        <c:crossAx val="123320192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -235,7 +263,159 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="ru-RU"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$A$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Последовательно</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1'!$A$8:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.7777777777777781E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7500000000000006E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7199074074074075E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$A$10:$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Параллельный внешний цикл</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1'!$A$17:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.1574074074074065E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2685185185185195E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8564814814814816E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1'!$A$19:$E$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Параллельный внутренний цикл</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1'!$A$26:$C$26</c:f>
+              <c:numCache>
+                <c:formatCode>mm:ss.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.6157407407407408E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4444444444444444E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.953703703703704E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="123294464"/>
+        <c:axId val="123296000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="123294464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="123296000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="123296000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="mm:ss.000" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="123294464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -245,16 +425,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -268,6 +448,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -563,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:Q1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -575,18 +785,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2">
@@ -606,113 +816,113 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>3.0092592592592594E-7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>3.7037037037037042E-7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>2.6851851851851852E-6</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>2.9018518518518515E-4</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>3.0092592592592594E-7</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>3.7037037037037042E-7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>2.7546296296296293E-6</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>2.8597222222222224E-4</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>2.6620370370370372E-7</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>3.8194444444444445E-7</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>2.7083333333333338E-6</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>2.8403935185185189E-4</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>2.6620370370370372E-7</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>3.7037037037037042E-7</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>2.7777777777777779E-6</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2.8603009259259255E-4</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>2.5462962962962963E-7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>3.8194444444444445E-7</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2.6736111111111111E-6</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2.8969907407407411E-4</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <f>AVERAGE(A3:A7)</f>
         <v>2.7777777777777781E-7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <f t="shared" ref="B8:E8" si="0">AVERAGE(B3:B7)</f>
         <v>3.7500000000000006E-7</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>2.7199074074074075E-6</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>2.8718518518518519E-4</v>
       </c>
-      <c r="E8" s="4" t="e">
+      <c r="E8" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:17">
       <c r="A11">
@@ -732,110 +942,110 @@
       </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>6.3657407407407403E-7</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>7.2916666666666664E-7</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>2.8935185185185184E-6</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>2.705787037037037E-4</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>6.3657407407407403E-7</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>7.1759259259259266E-7</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>2.8240740740740738E-6</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>2.7216435185185189E-4</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>6.2500000000000005E-7</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>7.4074074074074083E-7</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>2.8819444444444443E-6</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>2.7394675925925926E-4</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>5.9027777777777778E-7</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>7.1759259259259266E-7</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>2.8125000000000002E-6</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>2.7082175925925928E-4</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>5.9027777777777778E-7</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>7.2916666666666664E-7</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>2.8703703703703706E-6</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>2.7843749999999998E-4</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <f>AVERAGE(A12:A16)</f>
         <v>6.1574074074074065E-7</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <f t="shared" ref="B17:E17" si="1">AVERAGE(B12:B16)</f>
         <v>7.2685185185185195E-7</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f t="shared" si="1"/>
         <v>2.8564814814814816E-6</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <f t="shared" si="1"/>
         <v>2.7318981481481481E-4</v>
       </c>
-      <c r="E17" s="4" t="e">
+      <c r="E17" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
@@ -855,98 +1065,98 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>2.7777777777777776E-7</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>4.5138888888888888E-7</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>1.967592592592593E-6</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>1.3694444444444445E-4</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>2.5462962962962963E-7</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B22" s="3">
         <v>4.3981481481481479E-7</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>1.898148148148148E-6</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>1.3515046296296297E-4</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>2.6620370370370372E-7</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="3">
         <v>4.5138888888888888E-7</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>2.0138888888888885E-6</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>1.3872685185185187E-4</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>2.5462962962962963E-7</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="3">
         <v>4.3981481481481479E-7</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>1.9097222222222225E-6</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>1.4291666666666668E-4</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>2.5462962962962963E-7</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <v>4.3981481481481479E-7</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>1.9791666666666666E-6</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>1.4288194444444445E-4</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <f>AVERAGE(A21:A25)</f>
         <v>2.6157407407407408E-7</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <f t="shared" ref="B26:E26" si="2">AVERAGE(B21:B25)</f>
         <v>4.4444444444444444E-7</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <f t="shared" si="2"/>
         <v>1.953703703703704E-6</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <f t="shared" si="2"/>
         <v>1.393240740740741E-4</v>
       </c>
-      <c r="E26" s="4" t="e">
+      <c r="E26" s="3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>

</xml_diff>